<commit_message>
created an improved view for hospital variables
</commit_message>
<xml_diff>
--- a/src/main/resources/data/variables/Freiburg_v1.xlsx
+++ b/src/main/resources/data/variables/Freiburg_v1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t xml:space="preserve">csvFile</t>
   </si>
@@ -73,12 +73,18 @@
     <t xml:space="preserve">This column has no name initially</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/pet/av45</t>
+  </si>
+  <si>
     <t xml:space="preserve">PID_PSEUDONYMOUS</t>
   </si>
   <si>
     <t xml:space="preserve">text</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/pet/fdg</t>
+  </si>
+  <si>
     <t xml:space="preserve">SEX</t>
   </si>
   <si>
@@ -91,27 +97,42 @@
     <t xml:space="preserve">Gender: '0' for 'M', '1' for 'F'</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/pet/pib</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXAMINATION_DATE</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/brainstem</t>
+  </si>
+  <si>
     <t xml:space="preserve">YEAR_OF_BIRTH</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/tiv</t>
+  </si>
+  <si>
     <t xml:space="preserve">MMSE</t>
   </si>
   <si>
     <t xml:space="preserve">The Mini-Mental State Examination score</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/_3rdventricle</t>
+  </si>
+  <si>
     <t xml:space="preserve">DIAGNOSIS</t>
   </si>
   <si>
     <t xml:space="preserve">AD', 'MCI', 'LBD', 'FTD', 'VD', 'AD + VD', 'other'</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/_4thventricle</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_MEMORY</t>
   </si>
   <si>
@@ -124,30 +145,54 @@
     <t xml:space="preserve">Clinical Dementia Rating score https://en.wikipedia.org/wiki/Clinical_Dementia_Rating</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/csfglobal</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_ORIENTATION</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/leftinflatvent</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_JUDGMENT_AND_PROBLEM_SOLVING</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/leftlateralventricle</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_COMMUNITY_AFFAIRS</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/rightinflatvent</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_HOME_AND_HOBBIES</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/csf_volume/rightlateralventricle</t>
+  </si>
+  <si>
     <t xml:space="preserve">CDR_PERSONAL_CARE</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesiv</t>
+  </si>
+  <si>
     <t xml:space="preserve">GERIATRIC_DEPRESSION_SCALE</t>
   </si>
   <si>
     <t xml:space="preserve">The Geriatric Depression Scale (GDS) is a 30-item self-report assessment used to identify depression in the elderly. The scale was first developed in 1982 by J.A. Yesavage and others. https://en.wikipedia.org/wiki/Geriatric_Depression_Scale</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesviiix</t>
+  </si>
+  <si>
     <t xml:space="preserve">AGE</t>
   </si>
   <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/cerebellarvermallobulesvivii</t>
+  </si>
+  <si>
     <t xml:space="preserve">ALZHEIMER_BROAD_CATEGORY</t>
   </si>
   <si>
@@ -155,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">Alzheimer's Disease (AD) is when the diagnostic is 100% certain. Cognitively Normal (CN) subjects and "Other" comprising the rest of Alzheimer's related categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/root/brain_anatomy/grey_matter_volume/cerebellum/leftcerebellumexterior</t>
   </si>
 </sst>
 </file>
@@ -205,6 +253,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -321,16 +370,17 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="3" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -388,38 +438,47 @@
       <c r="I2" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="J3" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -427,11 +486,14 @@
         <v>11</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -439,26 +501,32 @@
         <v>11</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -466,14 +534,17 @@
         <v>11</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>35</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -481,20 +552,23 @@
         <v>11</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,20 +576,23 @@
         <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -523,20 +600,23 @@
         <v>11</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -544,20 +624,23 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,20 +648,23 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,20 +672,23 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,17 +696,20 @@
         <v>11</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -625,7 +717,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5" t="s">
@@ -634,23 +726,29 @@
       <c r="E16" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created a new view for the CDEs
</commit_message>
<xml_diff>
--- a/src/main/resources/data/variables/Freiburg_v1.xlsx
+++ b/src/main/resources/data/variables/Freiburg_v1.xlsx
@@ -370,17 +370,17 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="I24" activeCellId="0" sqref="I24:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.9591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>